<commit_message>
Refactoring a little bit the ExcelModel
</commit_message>
<xml_diff>
--- a/target/classes/cobigen-licenses-include.xlsx
+++ b/target/classes/cobigen-licenses-include.xlsx
@@ -2,27 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiazgon\Desktop\Contract_License\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" tabRatio="896"/>
   </bookViews>
   <sheets>
     <sheet name="SELECTION" sheetId="1" r:id="rId1"/>
     <sheet name="cobigen-core" sheetId="5" r:id="rId2"/>
     <sheet name="cobigen-eclipse" sheetId="6" r:id="rId3"/>
     <sheet name="cobigen-maven" sheetId="7" r:id="rId4"/>
+    <sheet name="cobigen-javaplugin" sheetId="9" r:id="rId5"/>
+    <sheet name="cobigen-propertyplugin" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="av_core">t_av_core[cobigen-core]</definedName>
     <definedName name="av_eclipse">t_av_eclipse[cobigen-eclipse]</definedName>
+    <definedName name="av_java">t_av_java[cobigen-javaplugin]</definedName>
     <definedName name="av_maven">t_av_maven[cobigen-maven]</definedName>
+    <definedName name="av_property">t_av_property[cobigen-propertyplugin]</definedName>
     <definedName name="languages">t_desc[Language]</definedName>
-    <definedName name="test">t_desc[Language]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
   <si>
     <t>cobigen-core</t>
   </si>
@@ -165,20 +168,86 @@
     <t>Embedded Components</t>
   </si>
   <si>
-    <t>Selected</t>
-  </si>
-  <si>
     <t>Main Applications</t>
   </si>
   <si>
-    <t>v.1.4.0</t>
+    <t>CobiGen Java Plug-in</t>
+  </si>
+  <si>
+    <t>QDox</t>
+  </si>
+  <si>
+    <t>2.0-M3</t>
+  </si>
+  <si>
+    <t>Mature Modular Meta-Framework (mmm-util-pojo)</t>
+  </si>
+  <si>
+    <t>cobigen-javaplugin</t>
+  </si>
+  <si>
+    <t>CobiGen Property Plug-in</t>
+  </si>
+  <si>
+    <t>v1.1.1</t>
+  </si>
+  <si>
+    <t>cobigen-propertyplugin</t>
+  </si>
+  <si>
+    <t>v2.1.0</t>
+  </si>
+  <si>
+    <t>Logback-classic</t>
+  </si>
+  <si>
+    <t>LGLP 2.1, EPL v1.0</t>
+  </si>
+  <si>
+    <t>Apache Ant</t>
+  </si>
+  <si>
+    <t>Apache Licence 2.0</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.9.6</t>
+  </si>
+  <si>
+    <t>v3.0.0</t>
+  </si>
+  <si>
+    <t>Maven-plugin-api</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Maven-core</t>
+  </si>
+  <si>
+    <t>Maven-compat</t>
+  </si>
+  <si>
+    <t>Maven-plugin-annotations</t>
+  </si>
+  <si>
+    <t>v1.6.0</t>
+  </si>
+  <si>
+    <t>v1.2.0</t>
+  </si>
+  <si>
+    <t>DE:Noch ein Kommentar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +289,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -296,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -347,15 +422,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="59">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -459,7 +562,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -563,17 +674,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -677,6 +784,226 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -724,126 +1051,182 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <tableColumns count="2">
-    <tableColumn id="1" name="Language" dataDxfId="31"/>
-    <tableColumn id="2" name="Description" dataDxfId="30"/>
+    <tableColumn id="1" name="Language" dataDxfId="56"/>
+    <tableColumn id="2" name="Description" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-maven" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="t_dep_java_150" displayName="t_dep_java_150" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="3"/>
-    <tableColumn id="2" name="Version" dataDxfId="2"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="1"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="21"/>
+    <tableColumn id="2" name="Version" dataDxfId="20"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B4:B6"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="t_dep_core_41013163" displayName="t_dep_core_41013163" ref="E17:G21" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="E17:G21"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="16"/>
+    <tableColumn id="2" name="Version" dataDxfId="15"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="t_av_java" displayName="t_av_java" ref="B4:B7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-maven"/>
+    <tableColumn id="1" name="cobigen-javaplugin" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="t_dep_java_1505" displayName="t_dep_java_1505" ref="E8:G9" totalsRowShown="0">
+  <autoFilter ref="E8:G9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="10"/>
+    <tableColumn id="2" name="Version" dataDxfId="9"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="t_dep_core_410131636" displayName="t_dep_core_410131636" ref="E15:G16" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="E15:G16"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="5"/>
+    <tableColumn id="2" name="Version" dataDxfId="4"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="t_av_property" displayName="t_av_property" ref="B4:B7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-propertyplugin" dataDxfId="0">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G17" totalsRowShown="0">
+  <autoFilter ref="E8:G17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="29"/>
-    <tableColumn id="2" name="Version" dataDxfId="28"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="27"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="54"/>
+    <tableColumn id="2" name="Version" dataDxfId="53"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G28" totalsRowShown="0" headerRowBorderDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="E20:G28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="24"/>
-    <tableColumn id="2" name="Version" dataDxfId="23"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="22"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="49"/>
+    <tableColumn id="2" name="Version" dataDxfId="48"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B6" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="B4:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+  <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-core"/>
+    <tableColumn id="1" name="cobigen-core" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="t_dep_core_40018" displayName="t_dep_core_40018" ref="K8:M16" totalsRowShown="0">
-  <autoFilter ref="K8:M16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="20">
-      <calculatedColumnFormula>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K9:$K$9)),1,1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="Version" dataDxfId="19"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="18"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="43"/>
+    <tableColumn id="2" name="Version" dataDxfId="42"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E17:G26" totalsRowShown="0" headerRowBorderDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="E17:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="17"/>
-    <tableColumn id="2" name="Version" dataDxfId="16"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="15"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="38"/>
+    <tableColumn id="2" name="Version" dataDxfId="37"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-eclipse" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="t_dep_core_4001215" displayName="t_dep_core_4001215" ref="E8:G14" totalsRowShown="0">
+  <autoFilter ref="E8:G14"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="12"/>
-    <tableColumn id="2" name="Version" dataDxfId="11"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="10"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="32"/>
+    <tableColumn id="2" name="Version" dataDxfId="31"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B6" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="B4:B6"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-eclipse"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="t_dep_core_4001215" displayName="t_dep_core_4001215" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G26" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="E20:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="8"/>
-    <tableColumn id="2" name="Version" dataDxfId="7"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="6"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="27"/>
+    <tableColumn id="2" name="Version" dataDxfId="26"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1115,14 +1498,14 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="18" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="18"/>
     <col min="6" max="6" width="9.7109375" style="18" customWidth="1"/>
     <col min="7" max="7" width="53.85546875" style="18" bestFit="1" customWidth="1"/>
@@ -1218,7 +1601,7 @@
     <row r="10" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -1236,7 +1619,7 @@
         <v>cobigen-eclipse</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21" t="str">
@@ -1255,7 +1638,7 @@
         <v>cobigen-maven</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21" t="str">
@@ -1336,15 +1719,18 @@
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
-      <c r="C18" s="21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="C18" s="21" t="str">
+        <f>t_av_java[[#Headers],[cobigen-javaplugin]]</f>
+        <v>cobigen-javaplugin</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="21" t="str">
+        <f>IF(D18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-javaplugin'!B2),"XXX",C18))</f>
+        <v>CobiGen Java Plug-in  (nachfolgend auch „cobigen-javaplugin“ genannt)</v>
+      </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -1352,15 +1738,18 @@
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
-      <c r="C19" s="21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="C19" s="21" t="str">
+        <f>t_av_property[[#Headers],[cobigen-propertyplugin]]</f>
+        <v>cobigen-propertyplugin</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21" t="str">
+        <f>IF(D19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-propertyplugin'!B2),"XXX",C19))</f>
+        <v>CobiGen Property Plug-in  (nachfolgend auch „cobigen-propertyplugin“ genannt)</v>
+      </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
@@ -1543,7 +1932,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
       <formula1>av_core</formula1>
     </dataValidation>
@@ -1557,7 +1946,10 @@
       <formula1>av_maven</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
-      <formula1>#REF!</formula1>
+      <formula1>av_java</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D19">
+      <formula1>av_property</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,16 +1962,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R31"/>
+  <dimension ref="B2:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -1594,7 +1986,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="16"/>
@@ -1605,31 +1997,29 @@
     </row>
     <row r="3" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v4.0.0</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D19</f>
+        <v>v4.1.0</v>
+      </c>
       <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="J7" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="J7" s="15"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -1643,15 +2033,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="15"/>
-      <c r="K8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E9" s="2" t="s">
@@ -1664,10 +2046,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="28"/>
-      <c r="K9" s="29" t="str">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K9:$K$9)),1,1)</f>
-        <v>SLF4J</v>
-      </c>
+      <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
@@ -1682,120 +2061,106 @@
         <v>10</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K10)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K11)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J12" s="15"/>
-      <c r="K12" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K12)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K12" s="29"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="K13" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K13)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K14)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K15)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K15" s="29"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K16)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K16" s="29"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
@@ -1806,10 +2171,7 @@
     <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
+      <c r="K18" s="3"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -1894,13 +2256,13 @@
     </row>
     <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -1914,13 +2276,13 @@
     </row>
     <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -1934,10 +2296,10 @@
     </row>
     <row r="25" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -1954,10 +2316,10 @@
     </row>
     <row r="26" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E26" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>10</v>
@@ -1974,10 +2336,10 @@
     </row>
     <row r="27" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>10</v>
@@ -1992,12 +2354,12 @@
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>10</v>
@@ -2012,16 +2374,7 @@
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
     </row>
-    <row r="29" spans="4:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>10</v>
-      </c>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
@@ -2043,25 +2396,13 @@
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2070,14 +2411,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -2090,7 +2431,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="16"/>
@@ -2101,18 +2442,14 @@
     </row>
     <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v2.1.0</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -2121,8 +2458,12 @@
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D16</f>
+        <v>v3.0.0</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2150,206 +2491,177 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E13" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E14" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G25" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
+    <row r="26" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G26" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>10</v>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
       </c>
     </row>
   </sheetData>
@@ -2367,14 +2679,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -2387,7 +2699,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="16"/>
@@ -2398,18 +2710,14 @@
     </row>
     <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v2.1.0</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -2418,8 +2726,12 @@
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D19</f>
+        <v>v3.0.0</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2447,32 +2759,32 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -2480,22 +2792,21 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
@@ -2503,29 +2814,22 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
+        <v>DE:Das CobiGen Maven Plug-in (cobigen-maven) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
+      <c r="E17" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
+        <v>EN:The CobiGen Maven Plug-in (cobigen-maven) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -2534,7 +2838,7 @@
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="15" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2563,43 +2867,43 @@
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E22" s="6" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -2607,7 +2911,7 @@
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E26" s="6" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>21</v>
@@ -2616,38 +2920,386 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="5" t="s">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Maven Plug-in (cobigen-maven) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Maven Plug-in (cobigen-maven) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.5.0</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="str">
+        <f>D16</f>
+        <v>v1.6.0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="7" t="s">
+    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="E13" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; B4 &amp; ")  wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Java Plug-in (cobigen-javaplugin)  wird gemeinsam mit cobigen-core ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="E14" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; B4 &amp; ") will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Java Plug-in (cobigen-javaplugin) will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="D16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G20" s="5" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.1.1</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="str">
+        <f>D14</f>
+        <v>v1.2.0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="E11" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; B4 &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Property Plug-in (cobigen-propertyplugin) wird gemeinsam mit cobigen-core ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="E12" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; B4 &amp; ") will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Property Plug-in (cobigen-propertyplugin) will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="D14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="E15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>